<commit_message>
Staré faktury by měly fungovat
</commit_message>
<xml_diff>
--- a/src/test/resources/test-old-invoices.xlsx
+++ b/src/test/resources/test-old-invoices.xlsx
@@ -12,15 +12,16 @@
     <sheet name="List3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Uhrazené faktury 2010'!$A$1:$S$10889</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Uhrazené faktury 2010'!$A$1:$S$10889</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Uhrazené faktury 2010'!$A$1:$S$10887</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Uhrazené faktury 2010'!$A$1:$S$10887</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Uhrazené faktury 2010'!$A$1:$S$10887</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="80">
   <si>
     <t>Číslo faktury</t>
   </si>
@@ -260,27 +261,6 @@
   </si>
   <si>
     <t>uveřejnění informace v IS</t>
-  </si>
-  <si>
-    <t>Auto FREIBERG</t>
-  </si>
-  <si>
-    <t>00803-01</t>
-  </si>
-  <si>
-    <t>mytí vozidel - Freiberg - 12/2009</t>
-  </si>
-  <si>
-    <t>Ochrana objektů se státní důležitostí s.r.o.</t>
-  </si>
-  <si>
-    <t>01146-01</t>
-  </si>
-  <si>
-    <t>FA 2009024</t>
-  </si>
-  <si>
-    <t>Ostraha objektu MF Lazarská 7 za 12/2009.                                                                                           Mandátní smlouva</t>
   </si>
 </sst>
 </file>
@@ -291,7 +271,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY\ H:MM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -313,13 +293,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -353,7 +326,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,10 +350,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -395,19 +364,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -421,10 +389,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1864,126 +1832,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>1000000027</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>2009004996</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>2009004996</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <v>2040</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="2" t="n">
-        <v>40178</v>
-      </c>
-      <c r="J25" s="2" t="n">
-        <v>40183.538912037</v>
-      </c>
-      <c r="K25" s="2" t="n">
-        <v>40192</v>
-      </c>
-      <c r="L25" s="2" t="n">
-        <v>40210</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>2040</v>
-      </c>
-      <c r="O25" s="0" t="n">
-        <v>2040</v>
-      </c>
-      <c r="P25" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R25" s="0" t="n">
-        <v>2040</v>
-      </c>
-      <c r="S25" s="0" t="n">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>1000000029</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>2009024</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <v>155778.5</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="2" t="n">
-        <v>40178</v>
-      </c>
-      <c r="J26" s="2" t="n">
-        <v>40183.5450462963</v>
-      </c>
-      <c r="K26" s="2" t="n">
-        <v>40192</v>
-      </c>
-      <c r="L26" s="2" t="n">
-        <v>40196</v>
-      </c>
-      <c r="M26" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="N26" s="0" t="n">
-        <v>155778.5</v>
-      </c>
-      <c r="O26" s="0" t="n">
-        <v>155778.5</v>
-      </c>
-      <c r="P26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R26" s="0" t="n">
-        <v>155778.5</v>
-      </c>
-      <c r="S26" s="0" t="n">
-        <v>155778.5</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:S10889"/>
+  <autoFilter ref="A1:S10887"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>